<commit_message>
Adding all setup files
Adding all previous setup files including comparison, default, and journal setups
</commit_message>
<xml_diff>
--- a/config/default.xlsx
+++ b/config/default.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schir\OneDrive\Studium\34_Github\PyPowerSim\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CFD138-A8F4-457C-ABFB-70510DDF0024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BD4CF4-A877-4909-81F4-E5A6CEB4DAD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{DB7D2548-4471-4992-93B1-3EC0BA66F7EA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{DB7D2548-4471-4992-93B1-3EC0BA66F7EA}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="237">
   <si>
     <t>#</t>
   </si>
@@ -780,6 +780,9 @@
   </si>
   <si>
     <t>0127</t>
+  </si>
+  <si>
+    <t>none</t>
   </si>
 </sst>
 </file>
@@ -1709,7 +1712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CAB857B-5D2E-4BE1-B462-B4B5EEAA4370}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -1789,7 +1792,7 @@
         <v>39</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>28</v>
+        <v>236</v>
       </c>
       <c r="F4" s="19" t="s">
         <v>23</v>
@@ -2534,7 +2537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245B3F0A-B85A-4162-A12D-AC7176B54015}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>

</xml_diff>